<commit_message>
Addition: imported files, added notes from tutorial
</commit_message>
<xml_diff>
--- a/week11/timetableData.xlsx
+++ b/week11/timetableData.xlsx
@@ -6417,224 +6417,224 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Powell, Blake</t>
+          <t>Harris, Jack</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Miller, Alison</t>
+          <t>Allan, Steven</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Howard, Faith</t>
+          <t>Harris, Lily</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Cornish, Nathan</t>
+          <t>Hardacre, Trevor</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Hamilton, Lisa</t>
+          <t>Carr, Isaac</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Jones, James</t>
+          <t>Burgess, Isaac</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Smith, Connor</t>
+          <t>Rutherford, Alexander</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MacLeod, Julia</t>
+          <t>Hamilton, Lisa</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Baker, Kevin</t>
+          <t>Cornish, Nathan</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Rutherford, Alexander</t>
+          <t>Terry, Sue</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Harris, Jack</t>
+          <t>Randall, Jason</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Paige, Jennifer</t>
+          <t>Jackson, Max</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Wilkins, Wendy</t>
+          <t>Baker, Kevin</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Harris, Lily</t>
+          <t>Smith, Connor</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Terry, Sue</t>
+          <t>Howard, Faith</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Marshall, Vanessa</t>
+          <t>Peters, Megan</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Carr, Isaac</t>
+          <t>Smith, Jonathan</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Hardacre, Trevor</t>
+          <t>BYRNE, JOHN (SHANE)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Duncan, Michelle</t>
+          <t>Miller, Alison</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Edmunds, Colin</t>
+          <t>Mackay, Claire</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Nolan, Stewart</t>
+          <t>Glover, Michael</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Peters, Megan</t>
+          <t>Marshall, Vanessa</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>BYRNE, JOHN (SHANE)</t>
+          <t>Jones, James</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Jackson, Max</t>
+          <t>Clarkson, Peter</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Edmunds, Madeleine</t>
+          <t>Edmunds, Colin</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Clarkson, Peter</t>
+          <t>Carr, Connor</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Mackay, Claire</t>
+          <t>Wilkins, Wendy</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Randall, Jason</t>
+          <t>Paige, Jennifer</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Burgess, Isaac</t>
+          <t>Powell, Blake</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Glover, Michael</t>
+          <t>Edmunds, Madeleine</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Carr, Connor</t>
+          <t>Nolan, Stewart</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Smith, Jonathan</t>
+          <t>Duncan, Michelle</t>
         </is>
       </c>
     </row>
@@ -6648,7 +6648,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Allan, Steven</t>
+          <t>MacLeod, Julia</t>
         </is>
       </c>
     </row>

</xml_diff>